<commit_message>
updated on Sep 10 2025
</commit_message>
<xml_diff>
--- a/AwesomeCV/data/main-data.xlsx
+++ b/AwesomeCV/data/main-data.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10916"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10817"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/myominnoo/Downloads/cv/AwesomeCV/data/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/myominnoo/Documents/GitHub/cv/AwesomeCV/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C72A718A-45B3-DF45-851D-BF7B8E63101B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F389E340-953F-6048-9BDA-EEE95221C5E7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="640" yWindow="760" windowWidth="33920" windowHeight="20760" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -32,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="624" uniqueCount="357">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="639" uniqueCount="363">
   <si>
     <t>Prince of Songkla University</t>
   </si>
@@ -743,9 +743,6 @@
   </si>
   <si>
     <t xml:space="preserve">Senior Research Associate </t>
-  </si>
-  <si>
-    <t>Apr 2024 - Present</t>
   </si>
   <si>
     <t>Oct 2023 - Mar 2024</t>
@@ -1104,6 +1101,27 @@
   </si>
   <si>
     <t>Postdoctoral Fellow</t>
+  </si>
+  <si>
+    <t>Apr 2024 - Apr 2025</t>
+  </si>
+  <si>
+    <t>Director of Research</t>
+  </si>
+  <si>
+    <t>Waapihk Research</t>
+  </si>
+  <si>
+    <t>May 2025 - Present</t>
+  </si>
+  <si>
+    <t>Direct multiple health and education projects at Waapihk Research, one of the largest Indigenous-led health economics firms.</t>
+  </si>
+  <si>
+    <t>Provide strategic research direction, oversee design and delivery, and ensure timely, high-quality outputs.</t>
+  </si>
+  <si>
+    <t>Lead and mentor a multidisciplinary team while representing the firm with clients, partners, and policymakers.</t>
   </si>
 </sst>
 </file>
@@ -2020,10 +2038,10 @@
     </row>
     <row r="2" spans="1:5" ht="48">
       <c r="A2" s="4" t="s">
-        <v>244</v>
+        <v>243</v>
       </c>
       <c r="B2" s="4" t="s">
-        <v>243</v>
+        <v>242</v>
       </c>
       <c r="C2" s="4" t="s">
         <v>0</v>
@@ -2037,10 +2055,10 @@
     </row>
     <row r="3" spans="1:5" ht="32">
       <c r="A3" s="4" t="s">
-        <v>244</v>
+        <v>243</v>
       </c>
       <c r="B3" s="4" t="s">
-        <v>243</v>
+        <v>242</v>
       </c>
       <c r="C3" s="4" t="s">
         <v>0</v>
@@ -2049,15 +2067,15 @@
         <v>1</v>
       </c>
       <c r="E3" s="4" t="s">
-        <v>245</v>
+        <v>244</v>
       </c>
     </row>
     <row r="4" spans="1:5" ht="32">
       <c r="A4" s="4" t="s">
-        <v>244</v>
+        <v>243</v>
       </c>
       <c r="B4" s="4" t="s">
-        <v>243</v>
+        <v>242</v>
       </c>
       <c r="C4" s="4" t="s">
         <v>0</v>
@@ -2066,15 +2084,15 @@
         <v>1</v>
       </c>
       <c r="E4" s="4" t="s">
-        <v>246</v>
+        <v>245</v>
       </c>
     </row>
     <row r="5" spans="1:5" ht="32">
       <c r="A5" s="4" t="s">
-        <v>244</v>
+        <v>243</v>
       </c>
       <c r="B5" s="4" t="s">
-        <v>243</v>
+        <v>242</v>
       </c>
       <c r="C5" s="4" t="s">
         <v>0</v>
@@ -2083,7 +2101,7 @@
         <v>1</v>
       </c>
       <c r="E5" s="4" t="s">
-        <v>247</v>
+        <v>246</v>
       </c>
     </row>
     <row r="6" spans="1:5" ht="80">
@@ -2108,7 +2126,7 @@
         <v>3</v>
       </c>
       <c r="B7" s="5" t="s">
-        <v>242</v>
+        <v>241</v>
       </c>
       <c r="C7" s="4" t="s">
         <v>2</v>
@@ -2117,7 +2135,7 @@
         <v>42</v>
       </c>
       <c r="E7" s="4" t="s">
-        <v>241</v>
+        <v>240</v>
       </c>
     </row>
   </sheetData>
@@ -2155,19 +2173,19 @@
     </row>
     <row r="2" spans="1:5">
       <c r="A2" t="s">
+        <v>332</v>
+      </c>
+      <c r="B2" t="s">
         <v>333</v>
       </c>
-      <c r="B2" t="s">
+      <c r="C2" t="s">
         <v>334</v>
       </c>
-      <c r="C2" t="s">
+      <c r="D2" t="s">
+        <v>238</v>
+      </c>
+      <c r="E2" t="s">
         <v>335</v>
-      </c>
-      <c r="D2" t="s">
-        <v>239</v>
-      </c>
-      <c r="E2" t="s">
-        <v>336</v>
       </c>
     </row>
     <row r="3" spans="1:5">
@@ -2178,13 +2196,13 @@
         <v>44743</v>
       </c>
       <c r="C3" t="s">
+        <v>337</v>
+      </c>
+      <c r="D3" t="s">
         <v>338</v>
       </c>
-      <c r="D3" t="s">
+      <c r="E3" t="s">
         <v>339</v>
-      </c>
-      <c r="E3" t="s">
-        <v>340</v>
       </c>
     </row>
     <row r="4" spans="1:5">
@@ -2201,7 +2219,7 @@
         <v>37</v>
       </c>
       <c r="E4" t="s">
-        <v>337</v>
+        <v>336</v>
       </c>
     </row>
     <row r="5" spans="1:5">
@@ -2346,16 +2364,16 @@
     </row>
     <row r="2" spans="1:5">
       <c r="A2" t="s">
-        <v>354</v>
+        <v>353</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>350</v>
+        <v>349</v>
       </c>
       <c r="C2" t="s">
-        <v>349</v>
+        <v>348</v>
       </c>
       <c r="D2" t="s">
-        <v>335</v>
+        <v>334</v>
       </c>
       <c r="E2" t="s">
         <v>28</v>
@@ -2363,7 +2381,7 @@
     </row>
     <row r="3" spans="1:5">
       <c r="A3" t="s">
-        <v>355</v>
+        <v>354</v>
       </c>
       <c r="B3" s="2" t="s">
         <v>220</v>
@@ -2375,7 +2393,7 @@
         <v>43</v>
       </c>
       <c r="E3" t="s">
-        <v>351</v>
+        <v>350</v>
       </c>
     </row>
     <row r="4" spans="1:5">
@@ -2389,10 +2407,10 @@
         <v>215</v>
       </c>
       <c r="D4" t="s">
-        <v>348</v>
+        <v>347</v>
       </c>
       <c r="E4" t="s">
-        <v>351</v>
+        <v>350</v>
       </c>
     </row>
     <row r="5" spans="1:5" ht="64">
@@ -2409,7 +2427,7 @@
         <v>0</v>
       </c>
       <c r="E5" t="s">
-        <v>352</v>
+        <v>351</v>
       </c>
     </row>
     <row r="6" spans="1:5">
@@ -2426,7 +2444,7 @@
         <v>0</v>
       </c>
       <c r="E6" t="s">
-        <v>352</v>
+        <v>351</v>
       </c>
     </row>
     <row r="7" spans="1:5">
@@ -2460,7 +2478,7 @@
         <v>228</v>
       </c>
       <c r="E8" t="s">
-        <v>353</v>
+        <v>352</v>
       </c>
     </row>
   </sheetData>
@@ -2479,10 +2497,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BE00790D-A8FD-D044-B711-36915F4C9436}">
-  <dimension ref="A1:E31"/>
+  <dimension ref="A1:E34"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A3" zoomScale="140" zoomScaleNormal="140" workbookViewId="0">
-      <selection activeCell="A12" sqref="A12"/>
+    <sheetView tabSelected="1" zoomScale="140" zoomScaleNormal="140" workbookViewId="0">
+      <selection activeCell="C9" sqref="C9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15"/>
@@ -2512,12 +2530,12 @@
         <v>8</v>
       </c>
     </row>
-    <row r="2" spans="1:5" ht="16">
+    <row r="2" spans="1:5" ht="32">
       <c r="A2" s="6" t="s">
-        <v>236</v>
+        <v>357</v>
       </c>
       <c r="B2" s="6" t="s">
-        <v>237</v>
+        <v>359</v>
       </c>
       <c r="C2" s="6" t="s">
         <v>341</v>
@@ -2526,15 +2544,15 @@
         <v>239</v>
       </c>
       <c r="E2" s="4" t="s">
-        <v>272</v>
-      </c>
-    </row>
-    <row r="3" spans="1:5" ht="32">
+        <v>360</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" ht="16">
       <c r="A3" s="6" t="s">
-        <v>236</v>
+        <v>357</v>
       </c>
       <c r="B3" s="6" t="s">
-        <v>237</v>
+        <v>359</v>
       </c>
       <c r="C3" s="6" t="s">
         <v>341</v>
@@ -2543,15 +2561,15 @@
         <v>239</v>
       </c>
       <c r="E3" s="4" t="s">
-        <v>273</v>
-      </c>
-    </row>
-    <row r="4" spans="1:5" ht="16">
+        <v>361</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" ht="32">
       <c r="A4" s="6" t="s">
-        <v>236</v>
+        <v>357</v>
       </c>
       <c r="B4" s="6" t="s">
-        <v>237</v>
+        <v>359</v>
       </c>
       <c r="C4" s="6" t="s">
         <v>341</v>
@@ -2560,131 +2578,131 @@
         <v>239</v>
       </c>
       <c r="E4" s="4" t="s">
-        <v>274</v>
-      </c>
-    </row>
-    <row r="5" spans="1:5" ht="32">
+        <v>362</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" ht="16">
       <c r="A5" s="6" t="s">
         <v>236</v>
       </c>
       <c r="B5" s="6" t="s">
-        <v>237</v>
+        <v>356</v>
       </c>
       <c r="C5" s="6" t="s">
-        <v>341</v>
+        <v>340</v>
       </c>
       <c r="D5" s="6" t="s">
-        <v>239</v>
+        <v>238</v>
       </c>
       <c r="E5" s="4" t="s">
-        <v>275</v>
+        <v>271</v>
       </c>
     </row>
     <row r="6" spans="1:5" ht="32">
       <c r="A6" s="6" t="s">
+        <v>236</v>
+      </c>
+      <c r="B6" s="6" t="s">
+        <v>356</v>
+      </c>
+      <c r="C6" s="6" t="s">
+        <v>340</v>
+      </c>
+      <c r="D6" s="6" t="s">
+        <v>238</v>
+      </c>
+      <c r="E6" s="4" t="s">
+        <v>272</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" ht="16">
+      <c r="A7" s="6" t="s">
+        <v>236</v>
+      </c>
+      <c r="B7" s="6" t="s">
+        <v>356</v>
+      </c>
+      <c r="C7" s="6" t="s">
+        <v>340</v>
+      </c>
+      <c r="D7" s="6" t="s">
+        <v>238</v>
+      </c>
+      <c r="E7" s="4" t="s">
+        <v>273</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5" ht="32">
+      <c r="A8" s="6" t="s">
+        <v>236</v>
+      </c>
+      <c r="B8" s="6" t="s">
+        <v>356</v>
+      </c>
+      <c r="C8" s="6" t="s">
+        <v>340</v>
+      </c>
+      <c r="D8" s="6" t="s">
+        <v>238</v>
+      </c>
+      <c r="E8" s="4" t="s">
+        <v>274</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5" ht="32">
+      <c r="A9" s="6" t="s">
         <v>235</v>
       </c>
-      <c r="B6" s="6" t="s">
-        <v>238</v>
-      </c>
-      <c r="C6" s="6" t="s">
-        <v>342</v>
-      </c>
-      <c r="D6" s="6" t="s">
-        <v>240</v>
-      </c>
-      <c r="E6" s="4" t="s">
+      <c r="B9" s="6" t="s">
+        <v>237</v>
+      </c>
+      <c r="C9" s="6" t="s">
+        <v>358</v>
+      </c>
+      <c r="D9" s="6" t="s">
+        <v>239</v>
+      </c>
+      <c r="E9" s="4" t="s">
+        <v>269</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5" ht="16" customHeight="1">
+      <c r="A10" s="6" t="s">
+        <v>235</v>
+      </c>
+      <c r="B10" s="6" t="s">
+        <v>237</v>
+      </c>
+      <c r="C10" s="6" t="s">
+        <v>358</v>
+      </c>
+      <c r="D10" s="6" t="s">
+        <v>239</v>
+      </c>
+      <c r="E10" s="4" t="s">
         <v>270</v>
       </c>
     </row>
-    <row r="7" spans="1:5" ht="16" customHeight="1">
-      <c r="A7" s="6" t="s">
+    <row r="11" spans="1:5" ht="16" customHeight="1">
+      <c r="A11" s="6" t="s">
         <v>235</v>
       </c>
-      <c r="B7" s="6" t="s">
-        <v>238</v>
-      </c>
-      <c r="C7" s="6" t="s">
-        <v>342</v>
-      </c>
-      <c r="D7" s="6" t="s">
-        <v>240</v>
-      </c>
-      <c r="E7" s="4" t="s">
-        <v>271</v>
-      </c>
-    </row>
-    <row r="8" spans="1:5" ht="16" customHeight="1">
-      <c r="A8" s="6" t="s">
-        <v>235</v>
-      </c>
-      <c r="B8" s="6" t="s">
-        <v>238</v>
-      </c>
-      <c r="C8" s="6" t="s">
-        <v>342</v>
-      </c>
-      <c r="D8" s="6" t="s">
-        <v>240</v>
-      </c>
-      <c r="E8" s="4" t="s">
-        <v>269</v>
-      </c>
-    </row>
-    <row r="9" spans="1:5" ht="16">
-      <c r="A9" s="6" t="s">
-        <v>356</v>
-      </c>
-      <c r="B9" s="6" t="s">
-        <v>234</v>
-      </c>
-      <c r="C9" s="6" t="s">
-        <v>43</v>
-      </c>
-      <c r="D9" s="6" t="s">
-        <v>240</v>
-      </c>
-      <c r="E9" s="4" t="s">
-        <v>265</v>
-      </c>
-    </row>
-    <row r="10" spans="1:5" ht="16">
-      <c r="A10" s="6" t="s">
-        <v>356</v>
-      </c>
-      <c r="B10" s="6" t="s">
-        <v>234</v>
-      </c>
-      <c r="C10" s="6" t="s">
-        <v>43</v>
-      </c>
-      <c r="D10" s="6" t="s">
-        <v>240</v>
-      </c>
-      <c r="E10" s="4" t="s">
-        <v>266</v>
-      </c>
-    </row>
-    <row r="11" spans="1:5" ht="32">
-      <c r="A11" s="6" t="s">
-        <v>356</v>
-      </c>
       <c r="B11" s="6" t="s">
-        <v>234</v>
+        <v>237</v>
       </c>
       <c r="C11" s="6" t="s">
-        <v>43</v>
+        <v>358</v>
       </c>
       <c r="D11" s="6" t="s">
-        <v>240</v>
+        <v>239</v>
       </c>
       <c r="E11" s="4" t="s">
-        <v>267</v>
-      </c>
-    </row>
-    <row r="12" spans="1:5" ht="32">
+        <v>268</v>
+      </c>
+    </row>
+    <row r="12" spans="1:5" ht="16">
       <c r="A12" s="6" t="s">
-        <v>356</v>
+        <v>355</v>
       </c>
       <c r="B12" s="6" t="s">
         <v>234</v>
@@ -2693,95 +2711,95 @@
         <v>43</v>
       </c>
       <c r="D12" s="6" t="s">
-        <v>240</v>
+        <v>239</v>
       </c>
       <c r="E12" s="4" t="s">
-        <v>268</v>
-      </c>
-    </row>
-    <row r="13" spans="1:5" ht="32">
+        <v>264</v>
+      </c>
+    </row>
+    <row r="13" spans="1:5" ht="16">
       <c r="A13" s="6" t="s">
+        <v>355</v>
+      </c>
+      <c r="B13" s="6" t="s">
+        <v>234</v>
+      </c>
+      <c r="C13" s="6" t="s">
+        <v>43</v>
+      </c>
+      <c r="D13" s="6" t="s">
+        <v>239</v>
+      </c>
+      <c r="E13" s="4" t="s">
+        <v>265</v>
+      </c>
+    </row>
+    <row r="14" spans="1:5" ht="32">
+      <c r="A14" s="6" t="s">
+        <v>355</v>
+      </c>
+      <c r="B14" s="6" t="s">
+        <v>234</v>
+      </c>
+      <c r="C14" s="6" t="s">
+        <v>43</v>
+      </c>
+      <c r="D14" s="6" t="s">
+        <v>239</v>
+      </c>
+      <c r="E14" s="4" t="s">
+        <v>266</v>
+      </c>
+    </row>
+    <row r="15" spans="1:5" ht="32">
+      <c r="A15" s="6" t="s">
+        <v>355</v>
+      </c>
+      <c r="B15" s="6" t="s">
+        <v>234</v>
+      </c>
+      <c r="C15" s="6" t="s">
+        <v>43</v>
+      </c>
+      <c r="D15" s="6" t="s">
+        <v>239</v>
+      </c>
+      <c r="E15" s="4" t="s">
+        <v>267</v>
+      </c>
+    </row>
+    <row r="16" spans="1:5" ht="32">
+      <c r="A16" s="6" t="s">
         <v>38</v>
-      </c>
-      <c r="B13" s="6" t="s">
-        <v>40</v>
-      </c>
-      <c r="C13" s="6" t="s">
-        <v>343</v>
-      </c>
-      <c r="D13" s="6" t="s">
-        <v>37</v>
-      </c>
-      <c r="E13" s="4" t="s">
-        <v>263</v>
-      </c>
-    </row>
-    <row r="14" spans="1:5" ht="16">
-      <c r="A14" s="6" t="s">
-        <v>38</v>
-      </c>
-      <c r="B14" s="6" t="s">
-        <v>40</v>
-      </c>
-      <c r="C14" s="6" t="s">
-        <v>343</v>
-      </c>
-      <c r="D14" s="6" t="s">
-        <v>37</v>
-      </c>
-      <c r="E14" s="4" t="s">
-        <v>264</v>
-      </c>
-    </row>
-    <row r="15" spans="1:5" ht="16">
-      <c r="A15" s="6" t="s">
-        <v>36</v>
-      </c>
-      <c r="B15" s="6" t="s">
-        <v>40</v>
-      </c>
-      <c r="C15" s="6" t="s">
-        <v>35</v>
-      </c>
-      <c r="D15" s="6" t="s">
-        <v>34</v>
-      </c>
-      <c r="E15" s="4" t="s">
-        <v>260</v>
-      </c>
-    </row>
-    <row r="16" spans="1:5" ht="16">
-      <c r="A16" s="6" t="s">
-        <v>36</v>
       </c>
       <c r="B16" s="6" t="s">
         <v>40</v>
       </c>
       <c r="C16" s="6" t="s">
-        <v>35</v>
+        <v>342</v>
       </c>
       <c r="D16" s="6" t="s">
-        <v>34</v>
+        <v>37</v>
       </c>
       <c r="E16" s="4" t="s">
-        <v>261</v>
+        <v>262</v>
       </c>
     </row>
     <row r="17" spans="1:5" ht="16">
       <c r="A17" s="6" t="s">
-        <v>36</v>
+        <v>38</v>
       </c>
       <c r="B17" s="6" t="s">
         <v>40</v>
       </c>
       <c r="C17" s="6" t="s">
-        <v>35</v>
+        <v>342</v>
       </c>
       <c r="D17" s="6" t="s">
-        <v>34</v>
+        <v>37</v>
       </c>
       <c r="E17" s="4" t="s">
-        <v>262</v>
+        <v>263</v>
       </c>
     </row>
     <row r="18" spans="1:5" ht="16">
@@ -2798,7 +2816,7 @@
         <v>34</v>
       </c>
       <c r="E18" s="4" t="s">
-        <v>54</v>
+        <v>259</v>
       </c>
     </row>
     <row r="19" spans="1:5" ht="16">
@@ -2815,112 +2833,112 @@
         <v>34</v>
       </c>
       <c r="E19" s="4" t="s">
+        <v>260</v>
+      </c>
+    </row>
+    <row r="20" spans="1:5" ht="16">
+      <c r="A20" s="6" t="s">
+        <v>36</v>
+      </c>
+      <c r="B20" s="6" t="s">
+        <v>40</v>
+      </c>
+      <c r="C20" s="6" t="s">
+        <v>35</v>
+      </c>
+      <c r="D20" s="6" t="s">
+        <v>34</v>
+      </c>
+      <c r="E20" s="4" t="s">
+        <v>261</v>
+      </c>
+    </row>
+    <row r="21" spans="1:5" ht="16">
+      <c r="A21" s="6" t="s">
+        <v>36</v>
+      </c>
+      <c r="B21" s="6" t="s">
+        <v>40</v>
+      </c>
+      <c r="C21" s="6" t="s">
+        <v>35</v>
+      </c>
+      <c r="D21" s="6" t="s">
+        <v>34</v>
+      </c>
+      <c r="E21" s="4" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="22" spans="1:5" ht="16">
+      <c r="A22" s="6" t="s">
+        <v>36</v>
+      </c>
+      <c r="B22" s="6" t="s">
+        <v>40</v>
+      </c>
+      <c r="C22" s="6" t="s">
+        <v>35</v>
+      </c>
+      <c r="D22" s="6" t="s">
+        <v>34</v>
+      </c>
+      <c r="E22" s="4" t="s">
         <v>55</v>
       </c>
     </row>
-    <row r="20" spans="1:5" ht="32">
-      <c r="A20" s="6" t="s">
+    <row r="23" spans="1:5" ht="32">
+      <c r="A23" s="6" t="s">
         <v>52</v>
       </c>
-      <c r="B20" s="6" t="s">
+      <c r="B23" s="6" t="s">
         <v>9</v>
       </c>
-      <c r="C20" s="6" t="s">
+      <c r="C23" s="6" t="s">
         <v>0</v>
       </c>
-      <c r="D20" s="6" t="s">
+      <c r="D23" s="6" t="s">
         <v>1</v>
       </c>
-      <c r="E20" s="4" t="s">
+      <c r="E23" s="4" t="s">
+        <v>256</v>
+      </c>
+    </row>
+    <row r="24" spans="1:5" ht="32">
+      <c r="A24" s="6" t="s">
+        <v>52</v>
+      </c>
+      <c r="B24" s="6" t="s">
+        <v>9</v>
+      </c>
+      <c r="C24" s="6" t="s">
+        <v>0</v>
+      </c>
+      <c r="D24" s="6" t="s">
+        <v>1</v>
+      </c>
+      <c r="E24" s="4" t="s">
         <v>257</v>
       </c>
     </row>
-    <row r="21" spans="1:5" ht="32">
-      <c r="A21" s="6" t="s">
+    <row r="25" spans="1:5" ht="32">
+      <c r="A25" s="6" t="s">
         <v>52</v>
       </c>
-      <c r="B21" s="6" t="s">
+      <c r="B25" s="6" t="s">
         <v>9</v>
       </c>
-      <c r="C21" s="6" t="s">
+      <c r="C25" s="6" t="s">
         <v>0</v>
       </c>
-      <c r="D21" s="6" t="s">
+      <c r="D25" s="6" t="s">
         <v>1</v>
       </c>
-      <c r="E21" s="4" t="s">
+      <c r="E25" s="4" t="s">
         <v>258</v>
       </c>
     </row>
-    <row r="22" spans="1:5" ht="32">
-      <c r="A22" s="6" t="s">
-        <v>52</v>
-      </c>
-      <c r="B22" s="6" t="s">
-        <v>9</v>
-      </c>
-      <c r="C22" s="6" t="s">
-        <v>0</v>
-      </c>
-      <c r="D22" s="6" t="s">
-        <v>1</v>
-      </c>
-      <c r="E22" s="4" t="s">
-        <v>259</v>
-      </c>
-    </row>
-    <row r="23" spans="1:5" ht="16">
-      <c r="A23" s="6" t="s">
-        <v>53</v>
-      </c>
-      <c r="B23" s="6" t="s">
-        <v>26</v>
-      </c>
-      <c r="C23" s="6" t="s">
-        <v>33</v>
-      </c>
-      <c r="D23" s="6" t="s">
-        <v>42</v>
-      </c>
-      <c r="E23" s="4" t="s">
-        <v>254</v>
-      </c>
-    </row>
-    <row r="24" spans="1:5" ht="16">
-      <c r="A24" s="6" t="s">
-        <v>53</v>
-      </c>
-      <c r="B24" s="6" t="s">
-        <v>26</v>
-      </c>
-      <c r="C24" s="6" t="s">
-        <v>33</v>
-      </c>
-      <c r="D24" s="6" t="s">
-        <v>42</v>
-      </c>
-      <c r="E24" s="4" t="s">
-        <v>255</v>
-      </c>
-    </row>
-    <row r="25" spans="1:5" ht="16">
-      <c r="A25" s="6" t="s">
-        <v>53</v>
-      </c>
-      <c r="B25" s="6" t="s">
-        <v>26</v>
-      </c>
-      <c r="C25" s="6" t="s">
-        <v>33</v>
-      </c>
-      <c r="D25" s="6" t="s">
-        <v>42</v>
-      </c>
-      <c r="E25" s="4" t="s">
-        <v>256</v>
-      </c>
-    </row>
-    <row r="26" spans="1:5" ht="32">
+    <row r="26" spans="1:5" ht="16">
       <c r="A26" s="6" t="s">
         <v>53</v>
       </c>
@@ -2934,66 +2952,66 @@
         <v>42</v>
       </c>
       <c r="E26" s="4" t="s">
-        <v>56</v>
-      </c>
-    </row>
-    <row r="27" spans="1:5" ht="32">
+        <v>253</v>
+      </c>
+    </row>
+    <row r="27" spans="1:5" ht="16">
       <c r="A27" s="6" t="s">
-        <v>39</v>
+        <v>53</v>
       </c>
       <c r="B27" s="6" t="s">
-        <v>32</v>
+        <v>26</v>
       </c>
       <c r="C27" s="6" t="s">
-        <v>30</v>
+        <v>33</v>
       </c>
       <c r="D27" s="6" t="s">
         <v>42</v>
       </c>
       <c r="E27" s="4" t="s">
-        <v>251</v>
-      </c>
-    </row>
-    <row r="28" spans="1:5" ht="32">
+        <v>254</v>
+      </c>
+    </row>
+    <row r="28" spans="1:5" ht="16">
       <c r="A28" s="6" t="s">
-        <v>39</v>
+        <v>53</v>
       </c>
       <c r="B28" s="6" t="s">
-        <v>32</v>
+        <v>26</v>
       </c>
       <c r="C28" s="6" t="s">
-        <v>30</v>
+        <v>33</v>
       </c>
       <c r="D28" s="6" t="s">
         <v>42</v>
       </c>
       <c r="E28" s="4" t="s">
-        <v>252</v>
+        <v>255</v>
       </c>
     </row>
     <row r="29" spans="1:5" ht="32">
       <c r="A29" s="6" t="s">
-        <v>39</v>
+        <v>53</v>
       </c>
       <c r="B29" s="6" t="s">
-        <v>32</v>
+        <v>26</v>
       </c>
       <c r="C29" s="6" t="s">
-        <v>30</v>
+        <v>33</v>
       </c>
       <c r="D29" s="6" t="s">
         <v>42</v>
       </c>
       <c r="E29" s="4" t="s">
-        <v>253</v>
+        <v>56</v>
       </c>
     </row>
     <row r="30" spans="1:5" ht="32">
       <c r="A30" s="6" t="s">
-        <v>248</v>
+        <v>39</v>
       </c>
       <c r="B30" s="6" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="C30" s="6" t="s">
         <v>30</v>
@@ -3002,15 +3020,15 @@
         <v>42</v>
       </c>
       <c r="E30" s="4" t="s">
-        <v>249</v>
+        <v>250</v>
       </c>
     </row>
     <row r="31" spans="1:5" ht="32">
       <c r="A31" s="6" t="s">
-        <v>248</v>
+        <v>39</v>
       </c>
       <c r="B31" s="6" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="C31" s="6" t="s">
         <v>30</v>
@@ -3019,7 +3037,58 @@
         <v>42</v>
       </c>
       <c r="E31" s="4" t="s">
-        <v>250</v>
+        <v>251</v>
+      </c>
+    </row>
+    <row r="32" spans="1:5" ht="32">
+      <c r="A32" s="6" t="s">
+        <v>39</v>
+      </c>
+      <c r="B32" s="6" t="s">
+        <v>32</v>
+      </c>
+      <c r="C32" s="6" t="s">
+        <v>30</v>
+      </c>
+      <c r="D32" s="6" t="s">
+        <v>42</v>
+      </c>
+      <c r="E32" s="4" t="s">
+        <v>252</v>
+      </c>
+    </row>
+    <row r="33" spans="1:5" ht="32">
+      <c r="A33" s="6" t="s">
+        <v>247</v>
+      </c>
+      <c r="B33" s="6" t="s">
+        <v>31</v>
+      </c>
+      <c r="C33" s="6" t="s">
+        <v>30</v>
+      </c>
+      <c r="D33" s="6" t="s">
+        <v>42</v>
+      </c>
+      <c r="E33" s="4" t="s">
+        <v>248</v>
+      </c>
+    </row>
+    <row r="34" spans="1:5" ht="32">
+      <c r="A34" s="6" t="s">
+        <v>247</v>
+      </c>
+      <c r="B34" s="6" t="s">
+        <v>31</v>
+      </c>
+      <c r="C34" s="6" t="s">
+        <v>30</v>
+      </c>
+      <c r="D34" s="6" t="s">
+        <v>42</v>
+      </c>
+      <c r="E34" s="4" t="s">
+        <v>249</v>
       </c>
     </row>
   </sheetData>
@@ -3060,36 +3129,36 @@
     </row>
     <row r="2" spans="1:5" ht="32">
       <c r="A2" t="s">
-        <v>277</v>
+        <v>276</v>
       </c>
       <c r="B2" t="s">
-        <v>279</v>
+        <v>278</v>
       </c>
       <c r="C2" s="3" t="s">
-        <v>344</v>
+        <v>343</v>
       </c>
       <c r="D2" t="s">
         <v>43</v>
       </c>
       <c r="E2" t="s">
-        <v>278</v>
+        <v>277</v>
       </c>
     </row>
     <row r="3" spans="1:5" ht="32">
       <c r="A3" t="s">
-        <v>277</v>
+        <v>276</v>
       </c>
       <c r="B3" t="s">
-        <v>279</v>
+        <v>278</v>
       </c>
       <c r="C3" s="3" t="s">
-        <v>344</v>
+        <v>343</v>
       </c>
       <c r="D3" t="s">
         <v>43</v>
       </c>
       <c r="E3" t="s">
-        <v>280</v>
+        <v>279</v>
       </c>
     </row>
     <row r="4" spans="1:5">
@@ -3174,7 +3243,7 @@
         <v>14</v>
       </c>
       <c r="E8" t="s">
-        <v>276</v>
+        <v>275</v>
       </c>
     </row>
     <row r="9" spans="1:5">
@@ -3244,7 +3313,7 @@
     </row>
     <row r="2" spans="1:3">
       <c r="A2" t="s">
-        <v>292</v>
+        <v>291</v>
       </c>
       <c r="B2" t="s">
         <v>133</v>
@@ -3255,13 +3324,13 @@
     </row>
     <row r="3" spans="1:3">
       <c r="A3" t="s">
+        <v>291</v>
+      </c>
+      <c r="B3" t="s">
         <v>292</v>
       </c>
-      <c r="B3" t="s">
+      <c r="C3" t="s">
         <v>293</v>
-      </c>
-      <c r="C3" t="s">
-        <v>294</v>
       </c>
     </row>
     <row r="4" spans="1:3">
@@ -3305,7 +3374,7 @@
         <v>147</v>
       </c>
       <c r="C7" t="s">
-        <v>284</v>
+        <v>283</v>
       </c>
     </row>
     <row r="8" spans="1:3">
@@ -3316,7 +3385,7 @@
         <v>148</v>
       </c>
       <c r="C8" t="s">
-        <v>285</v>
+        <v>284</v>
       </c>
     </row>
     <row r="9" spans="1:3">
@@ -3364,7 +3433,7 @@
         <v>141</v>
       </c>
       <c r="B14" t="s">
-        <v>307</v>
+        <v>306</v>
       </c>
     </row>
     <row r="15" spans="1:3">
@@ -3408,12 +3477,12 @@
         <v>152</v>
       </c>
       <c r="C18" t="s">
-        <v>295</v>
+        <v>294</v>
       </c>
     </row>
     <row r="19" spans="1:3">
       <c r="A19" t="s">
-        <v>286</v>
+        <v>285</v>
       </c>
       <c r="B19" t="s">
         <v>45</v>
@@ -3421,10 +3490,10 @@
     </row>
     <row r="20" spans="1:3">
       <c r="A20" t="s">
+        <v>285</v>
+      </c>
+      <c r="B20" t="s">
         <v>286</v>
-      </c>
-      <c r="B20" t="s">
-        <v>287</v>
       </c>
     </row>
     <row r="21" spans="1:3">
@@ -3440,10 +3509,10 @@
         <v>136</v>
       </c>
       <c r="B22" t="s">
+        <v>289</v>
+      </c>
+      <c r="C22" t="s">
         <v>290</v>
-      </c>
-      <c r="C22" t="s">
-        <v>291</v>
       </c>
     </row>
     <row r="23" spans="1:3">
@@ -3491,7 +3560,7 @@
         <v>136</v>
       </c>
       <c r="B28" t="s">
-        <v>283</v>
+        <v>282</v>
       </c>
     </row>
     <row r="29" spans="1:3">
@@ -3582,24 +3651,24 @@
     </row>
     <row r="39" spans="1:3">
       <c r="A39" t="s">
-        <v>282</v>
+        <v>281</v>
       </c>
       <c r="B39" t="s">
+        <v>287</v>
+      </c>
+      <c r="C39" t="s">
         <v>288</v>
-      </c>
-      <c r="C39" t="s">
-        <v>289</v>
       </c>
     </row>
     <row r="40" spans="1:3">
       <c r="A40" t="s">
-        <v>281</v>
+        <v>280</v>
       </c>
       <c r="B40" t="s">
-        <v>306</v>
+        <v>305</v>
       </c>
       <c r="C40" t="s">
-        <v>305</v>
+        <v>304</v>
       </c>
     </row>
     <row r="41" spans="1:3">
@@ -3671,7 +3740,7 @@
         <v>160</v>
       </c>
       <c r="B49" t="s">
-        <v>296</v>
+        <v>295</v>
       </c>
     </row>
     <row r="50" spans="1:2">
@@ -3740,7 +3809,7 @@
         <v>168</v>
       </c>
       <c r="B4" t="s">
-        <v>297</v>
+        <v>296</v>
       </c>
       <c r="C4" t="s">
         <v>203</v>
@@ -3751,7 +3820,7 @@
         <v>174</v>
       </c>
       <c r="B5" t="s">
-        <v>298</v>
+        <v>297</v>
       </c>
       <c r="C5" t="s">
         <v>43</v>
@@ -3762,7 +3831,7 @@
         <v>175</v>
       </c>
       <c r="B6" t="s">
-        <v>299</v>
+        <v>298</v>
       </c>
       <c r="C6" t="s">
         <v>67</v>
@@ -3773,7 +3842,7 @@
         <v>167</v>
       </c>
       <c r="B7" t="s">
-        <v>300</v>
+        <v>299</v>
       </c>
       <c r="C7" t="s">
         <v>171</v>
@@ -3784,7 +3853,7 @@
         <v>167</v>
       </c>
       <c r="B8" t="s">
-        <v>300</v>
+        <v>299</v>
       </c>
       <c r="C8" t="s">
         <v>170</v>
@@ -3795,7 +3864,7 @@
         <v>169</v>
       </c>
       <c r="B9" t="s">
-        <v>301</v>
+        <v>300</v>
       </c>
       <c r="C9" t="s">
         <v>0</v>
@@ -3806,10 +3875,10 @@
         <v>28</v>
       </c>
       <c r="B10" t="s">
-        <v>304</v>
+        <v>303</v>
       </c>
       <c r="C10" t="s">
-        <v>303</v>
+        <v>302</v>
       </c>
     </row>
     <row r="11" spans="1:3">
@@ -3836,7 +3905,7 @@
     </row>
     <row r="13" spans="1:3">
       <c r="A13" t="s">
-        <v>302</v>
+        <v>301</v>
       </c>
       <c r="B13" t="s">
         <v>23</v>
@@ -3847,7 +3916,7 @@
     </row>
     <row r="14" spans="1:3">
       <c r="A14" t="s">
-        <v>302</v>
+        <v>301</v>
       </c>
       <c r="B14" t="s">
         <v>23</v>
@@ -3858,7 +3927,7 @@
     </row>
     <row r="15" spans="1:3">
       <c r="A15" t="s">
-        <v>302</v>
+        <v>301</v>
       </c>
       <c r="B15" t="s">
         <v>23</v>
@@ -3869,7 +3938,7 @@
     </row>
     <row r="16" spans="1:3">
       <c r="A16" t="s">
-        <v>302</v>
+        <v>301</v>
       </c>
       <c r="B16" t="s">
         <v>23</v>
@@ -3880,7 +3949,7 @@
     </row>
     <row r="17" spans="1:3">
       <c r="A17" t="s">
-        <v>302</v>
+        <v>301</v>
       </c>
       <c r="B17" t="s">
         <v>23</v>
@@ -3891,7 +3960,7 @@
     </row>
     <row r="18" spans="1:3">
       <c r="A18" t="s">
-        <v>302</v>
+        <v>301</v>
       </c>
       <c r="B18" t="s">
         <v>23</v>
@@ -3902,7 +3971,7 @@
     </row>
     <row r="19" spans="1:3">
       <c r="A19" t="s">
-        <v>302</v>
+        <v>301</v>
       </c>
       <c r="B19" t="s">
         <v>23</v>
@@ -3913,7 +3982,7 @@
     </row>
     <row r="20" spans="1:3">
       <c r="A20" t="s">
-        <v>302</v>
+        <v>301</v>
       </c>
       <c r="B20" t="s">
         <v>23</v>
@@ -3924,7 +3993,7 @@
     </row>
     <row r="21" spans="1:3">
       <c r="A21" t="s">
-        <v>302</v>
+        <v>301</v>
       </c>
       <c r="B21" t="s">
         <v>23</v>
@@ -3975,10 +4044,10 @@
         <v>176</v>
       </c>
       <c r="B2" t="s">
-        <v>312</v>
+        <v>311</v>
       </c>
       <c r="C2" t="s">
-        <v>345</v>
+        <v>344</v>
       </c>
       <c r="D2" s="2" t="s">
         <v>178</v>
@@ -3992,10 +4061,10 @@
         <v>191</v>
       </c>
       <c r="B3" t="s">
-        <v>313</v>
+        <v>312</v>
       </c>
       <c r="C3" t="s">
-        <v>345</v>
+        <v>344</v>
       </c>
       <c r="D3" s="2" t="s">
         <v>193</v>
@@ -4006,34 +4075,34 @@
     </row>
     <row r="4" spans="1:5">
       <c r="A4" t="s">
+        <v>309</v>
+      </c>
+      <c r="B4" t="s">
         <v>310</v>
       </c>
-      <c r="B4" t="s">
-        <v>311</v>
-      </c>
       <c r="C4" t="s">
-        <v>345</v>
+        <v>344</v>
       </c>
       <c r="D4" s="2" t="s">
-        <v>308</v>
+        <v>307</v>
       </c>
       <c r="E4" s="2"/>
     </row>
     <row r="5" spans="1:5">
       <c r="A5" t="s">
+        <v>318</v>
+      </c>
+      <c r="B5" t="s">
         <v>319</v>
       </c>
-      <c r="B5" t="s">
+      <c r="C5" t="s">
+        <v>315</v>
+      </c>
+      <c r="D5" s="2" t="s">
+        <v>321</v>
+      </c>
+      <c r="E5" s="2" t="s">
         <v>320</v>
-      </c>
-      <c r="C5" t="s">
-        <v>316</v>
-      </c>
-      <c r="D5" s="2" t="s">
-        <v>322</v>
-      </c>
-      <c r="E5" s="2" t="s">
-        <v>321</v>
       </c>
     </row>
     <row r="6" spans="1:5">
@@ -4044,7 +4113,7 @@
         <v>194</v>
       </c>
       <c r="C6" t="s">
-        <v>316</v>
+        <v>315</v>
       </c>
       <c r="D6" s="2" t="s">
         <v>189</v>
@@ -4056,10 +4125,10 @@
         <v>188</v>
       </c>
       <c r="B7" t="s">
-        <v>346</v>
+        <v>345</v>
       </c>
       <c r="C7" t="s">
-        <v>316</v>
+        <v>315</v>
       </c>
       <c r="D7" s="2" t="s">
         <v>190</v>
@@ -4071,10 +4140,10 @@
         <v>196</v>
       </c>
       <c r="B8" t="s">
-        <v>323</v>
+        <v>322</v>
       </c>
       <c r="C8" t="s">
-        <v>316</v>
+        <v>315</v>
       </c>
       <c r="D8" s="2" t="s">
         <v>195</v>
@@ -4083,13 +4152,13 @@
     </row>
     <row r="9" spans="1:5">
       <c r="A9" t="s">
-        <v>314</v>
+        <v>313</v>
       </c>
       <c r="B9" t="s">
         <v>183</v>
       </c>
       <c r="C9" t="s">
-        <v>315</v>
+        <v>314</v>
       </c>
       <c r="D9" s="2" t="s">
         <v>179</v>
@@ -4106,7 +4175,7 @@
         <v>185</v>
       </c>
       <c r="C10" t="s">
-        <v>309</v>
+        <v>308</v>
       </c>
       <c r="D10" s="2" t="s">
         <v>180</v>
@@ -4117,46 +4186,46 @@
     </row>
     <row r="11" spans="1:5">
       <c r="A11" t="s">
+        <v>323</v>
+      </c>
+      <c r="B11" t="s">
         <v>324</v>
       </c>
-      <c r="B11" t="s">
+      <c r="C11" t="s">
+        <v>308</v>
+      </c>
+      <c r="D11" s="2" t="s">
         <v>325</v>
-      </c>
-      <c r="C11" t="s">
-        <v>309</v>
-      </c>
-      <c r="D11" s="2" t="s">
-        <v>326</v>
       </c>
       <c r="E11" s="2"/>
     </row>
     <row r="12" spans="1:5">
       <c r="A12" t="s">
+        <v>326</v>
+      </c>
+      <c r="B12" t="s">
         <v>327</v>
       </c>
-      <c r="B12" t="s">
+      <c r="C12" t="s">
+        <v>308</v>
+      </c>
+      <c r="D12" s="2" t="s">
         <v>328</v>
-      </c>
-      <c r="C12" t="s">
-        <v>309</v>
-      </c>
-      <c r="D12" s="2" t="s">
-        <v>329</v>
       </c>
       <c r="E12" s="2"/>
     </row>
     <row r="13" spans="1:5">
       <c r="A13" t="s">
+        <v>316</v>
+      </c>
+      <c r="B13" t="s">
+        <v>346</v>
+      </c>
+      <c r="C13" t="s">
+        <v>314</v>
+      </c>
+      <c r="D13" s="2" t="s">
         <v>317</v>
-      </c>
-      <c r="B13" t="s">
-        <v>347</v>
-      </c>
-      <c r="C13" t="s">
-        <v>315</v>
-      </c>
-      <c r="D13" s="2" t="s">
-        <v>318</v>
       </c>
       <c r="E13" s="2" t="s">
         <v>186</v>
@@ -4200,7 +4269,7 @@
     </row>
     <row r="2" spans="1:7">
       <c r="A2" t="s">
-        <v>331</v>
+        <v>330</v>
       </c>
     </row>
     <row r="3" spans="1:7">
@@ -4210,7 +4279,7 @@
     </row>
     <row r="4" spans="1:7">
       <c r="A4" t="s">
-        <v>330</v>
+        <v>329</v>
       </c>
     </row>
     <row r="5" spans="1:7">
@@ -4220,7 +4289,7 @@
     </row>
     <row r="6" spans="1:7">
       <c r="A6" t="s">
-        <v>332</v>
+        <v>331</v>
       </c>
     </row>
     <row r="10" spans="1:7">

</xml_diff>